<commit_message>
add avaliações para Results_Tfidf
</commit_message>
<xml_diff>
--- a/reviews/Results_Bm25_Vanessa.xlsx
+++ b/reviews/Results_Bm25_Vanessa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanes\OneDrive\Área de Trabalho\Projetos em CD\Search_Engine\reviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B96F141-C7C5-4EBD-BC01-F508F44FD679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DDC5B4-81A2-4A6A-AD4A-7396A2ECE8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2664,7 +2664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2971,8 +2971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F221" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="F55" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3161,7 +3161,7 @@
         <v>30</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
@@ -3253,7 +3253,7 @@
         <v>42</v>
       </c>
       <c r="G12">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
@@ -3322,7 +3322,7 @@
         <v>51</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">

</xml_diff>